<commit_message>
Update to demo file
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-V2-original-noID.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-V2-original-noID.xlsx
@@ -811,7 +811,9 @@
   </sheetPr>
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1118,7 +1120,7 @@
     </row>
     <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C6" s="6">
         <v>1311525</v>
@@ -1290,7 +1292,7 @@
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C9" s="6">
         <v>1311528</v>

</xml_diff>

<commit_message>
Add updates to mapping/merging for demo
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-V2-original-noID.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-V2-original-noID.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -56,9 +56,6 @@
     <t>address_line_1</t>
   </si>
   <si>
-    <t>jurisdiction_property_identifier</t>
-  </si>
-  <si>
     <t>Case A-1: 1 Property, 1 Tax Lot</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>295302 Moser Lane</t>
   </si>
   <si>
-    <t>05840022, 06490020</t>
-  </si>
-  <si>
     <t>City Library</t>
   </si>
   <si>
@@ -297,6 +291,9 @@
   </si>
   <si>
     <t>custom_id_1</t>
+  </si>
+  <si>
+    <t>jurisdiction_property_id</t>
   </si>
 </sst>
 </file>
@@ -414,7 +411,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -439,6 +436,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="36">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -812,7 +810,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -836,31 +834,31 @@
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>4</v>
@@ -875,22 +873,22 @@
         <v>8</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T1" s="4"/>
     </row>
@@ -903,19 +901,19 @@
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="7">
         <v>1552813</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" s="7">
         <v>75</v>
@@ -930,19 +928,19 @@
         <v>12555</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="S2" s="7">
         <v>1</v>
@@ -958,19 +956,19 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="G3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="7">
         <v>11160509</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" s="7">
         <v>63</v>
@@ -985,19 +983,19 @@
         <v>23543</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S3" s="7">
         <v>4</v>
@@ -1015,46 +1013,46 @@
         <v>1311523</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="7">
         <v>24651456</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4" s="8">
         <v>42369</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S4" s="7">
         <v>6</v>
@@ -1072,19 +1070,19 @@
         <v>1311523</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" s="7">
         <v>24651456</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J5" s="7">
         <v>77</v>
@@ -1099,19 +1097,19 @@
         <v>124523</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="S5" s="7">
         <v>7</v>
@@ -1129,19 +1127,19 @@
         <v>1311523</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" s="7">
         <v>24651456</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" s="7">
         <v>43</v>
@@ -1156,19 +1154,19 @@
         <v>421351</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="S6" s="7">
         <v>8</v>
@@ -1187,19 +1185,19 @@
         <v>1311523</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" s="7">
         <v>24651456</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="7">
         <v>59</v>
@@ -1214,19 +1212,19 @@
         <v>1234</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="S7" s="7">
         <v>9</v>
@@ -1244,19 +1242,19 @@
         <v>1311523</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="J8" s="7">
         <v>34</v>
@@ -1271,19 +1269,19 @@
         <v>45324</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="S8" s="7">
         <v>10</v>
@@ -1301,25 +1299,25 @@
         <v>1311523</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="G9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="K9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L9" s="8">
         <v>42369</v>
@@ -1328,19 +1326,19 @@
         <v>482215</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="S9" s="7">
         <v>11</v>
@@ -1356,19 +1354,19 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H10" s="7">
         <v>11160509</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J10" s="7">
         <v>1</v>
@@ -1383,19 +1381,19 @@
         <v>513852</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S10" s="7">
         <v>2</v>
@@ -1412,25 +1410,25 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H11" s="7">
         <v>11160509</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L11" s="8">
         <v>42369</v>
@@ -1439,19 +1437,19 @@
         <v>55121</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S11" s="7">
         <v>3</v>
@@ -1468,19 +1466,19 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>1</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J12" s="7">
         <v>55</v>
@@ -1495,19 +1493,19 @@
         <v>200000</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S12" s="7">
         <v>5</v>
@@ -1522,19 +1520,19 @@
         <v>6798215</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="16">
+        <v>13334485</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="J13" s="7">
         <v>88</v>
@@ -1549,19 +1547,19 @@
         <v>24523</v>
       </c>
       <c r="N13" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P13" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="O13" s="12" t="s">
+      <c r="Q13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="P13" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>72</v>
-      </c>
       <c r="R13" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S13" s="7">
         <v>12</v>

</xml_diff>